<commit_message>
Merge SpellShaping mod into archid
The spell shaping mod had a few minor bugs included in the script files so needed to be merged into the archid mod in order to recompile them.
As part of this process the changes to update dains fixes were also merged in, including both the event manager and effect manager.
The gda file entries from dains fixes that would have been overridden due to load order were removed to simplify the files.
</commit_message>
<xml_diff>
--- a/source/strings.xlsx
+++ b/source/strings.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid_mod\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9714F9B7-1A2A-4F9C-8569-28E11C3C997D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FCF121-96D4-4010-B0F5-94FC5322B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="3675" windowWidth="21990" windowHeight="13635" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="840" yWindow="990" windowWidth="20625" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$470</definedName>
+    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$473</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="906">
   <si>
     <t>C:/Users/Jim/Documents/BioWare/Dragon Age/addins/af_archid/module/override/</t>
   </si>
@@ -2788,6 +2788,15 @@
   <si>
     <t>&lt;emp&gt;Lothering is lost&lt;/emp&gt;
 Lothering has been overrun by darkspawn. You do not know whether Ser Arbither Cora has perished or escaped; whatever happened, she did it without your help.</t>
+  </si>
+  <si>
+    <t>6610005</t>
+  </si>
+  <si>
+    <t>6610006</t>
+  </si>
+  <si>
+    <t>6610007</t>
   </si>
 </sst>
 </file>
@@ -3150,11 +3159,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D158D-1FBF-4946-A52B-028752432AE5}">
-  <dimension ref="A1:B470"/>
+  <dimension ref="A1:B473"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,3729 +3212,3753 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>662</v>
+        <v>903</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>664</v>
+        <v>904</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>666</v>
+        <v>905</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>667</v>
+        <v>886</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>891</v>
+        <v>667</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>678</v>
+        <v>891</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>892</v>
+        <v>676</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>893</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>897</v>
+        <v>691</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>699</v>
+        <v>897</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>702</v>
+        <v>899</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>665</v>
+        <v>900</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>711</v>
+        <v>665</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>638</v>
+        <v>707</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>640</v>
+        <v>709</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>272</v>
+        <v>711</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>274</v>
+        <v>638</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>717</v>
+        <v>640</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>719</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>721</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>283</v>
+        <v>765</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>285</v>
+        <v>767</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>775</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>782</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>293</v>
+        <v>784</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>293</v>
+        <v>786</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>735</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>737</v>
+        <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>632</v>
+        <v>735</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>799</v>
+        <v>737</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>647</v>
+        <v>796</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>890</v>
+        <v>798</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>805</v>
+        <v>647</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>901</v>
+        <v>803</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>287</v>
+        <v>805</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>812</v>
+        <v>901</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>902</v>
+        <v>810</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>293</v>
+        <v>812</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>820</v>
+        <v>902</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>822</v>
+        <v>293</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>71</v>
+        <v>842</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>853</v>
+        <v>71</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>71</v>
+        <v>855</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>289</v>
+        <v>857</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>865</v>
+        <v>71</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>867</v>
+        <v>289</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>685</v>
+        <v>871</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>125</v>
+        <v>876</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>146</v>
+        <v>877</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>147</v>
+        <v>878</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>136</v>
+        <v>879</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>137</v>
+        <v>880</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>251</v>
+        <v>135</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>252</v>
+        <v>126</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>253</v>
+        <v>142</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>254</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>255</v>
+        <v>144</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>256</v>
+        <v>145</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="B347" s="3" t="s">
-        <v>890</v>
+        <v>637</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="B350" s="2" t="s">
-        <v>649</v>
+        <v>643</v>
+      </c>
+      <c r="B350" s="3" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>214</v>
+        <v>656</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>215</v>
+        <v>657</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>216</v>
+        <v>658</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>218</v>
+        <v>660</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>219</v>
+        <v>661</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>889</v>
+        <v>241</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>101</v>
+        <v>889</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>102</v>
+        <v>247</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>103</v>
+        <v>248</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>104</v>
+        <v>249</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>105</v>
+        <v>250</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="380" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>886</v>
+        <v>103</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>114</v>
+        <v>886</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>888</v>
+        <v>118</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="390" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>82</v>
+        <v>888</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="394" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>882</v>
+        <v>82</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>63</v>
+        <v>882</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B409" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="B413" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B415" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="416" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B417" s="2" t="s">
-        <v>885</v>
+        <v>73</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>24</v>
+        <v>885</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B423" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B429" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B435" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B438" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B439" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B440" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B438" s="2" t="s">
+      <c r="B441" s="2" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A439" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B439" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A440" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B440" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="441" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A441" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B441" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B443" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B445" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B449" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B451" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="452" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B453" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B455" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B459" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B465" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B467" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B468" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B469" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A470" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B470" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B468" s="2" t="s">
+      <c r="B471" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="469" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A469" s="1" t="s">
+    <row r="472" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A472" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B469" s="2" t="s">
+      <c r="B472" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A470" s="1" t="s">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B470" s="2" t="s">
+      <c r="B473" s="2" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B470">
-    <sortCondition ref="A2:A470"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B473">
+    <sortCondition ref="A2:A473"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Merge Shale Talents Reworked mod
This mod has a custom core_h file and a recompiled rules_core. Merged the mod to ensure that all code has the same libraries included. The commit also contains other scripts that have been recompiled against the new library code.
</commit_message>
<xml_diff>
--- a/source/strings.xlsx
+++ b/source/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid_mod\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343B207B-728A-4A55-92EB-C022FCD6B889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE0F26-3EF4-4E59-B365-4C6818977C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29145" yWindow="1710" windowWidth="24540" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="615" yWindow="1350" windowWidth="18780" windowHeight="15645" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,199 +439,100 @@
     <t>When active, the caster will shape and direct wide-area spells to avoid friendly fire at a cost of additional mana. Party members gain protection from the damage, with the additional mana spent based on the number of allies in the target area.</t>
   </si>
   <si>
-    <t>1602176565</t>
-  </si>
-  <si>
     <t>Shale activates a mode that focuses on offense, taking penalties to defense and armor in exchange for bonuses to damage and attack. Slam, Quake, and Killing Blow add bonuses to this mode.</t>
   </si>
   <si>
-    <t>1602176566</t>
-  </si>
-  <si>
     <t>Shale slams a stony fist into the enemy target. If the blow connects, it generates an automatic critical hit and knocks the target back. The target is also stunned briefly unless it passes a physical resistance check. After learning this talent, Shale gains bonuses to damage, attack, and armor penetration whenever Pulverizing Blows is active.</t>
   </si>
   <si>
-    <t>1602176567</t>
-  </si>
-  <si>
     <t>Shale strikes the ground repeatedly, sending out multiple shockwaves. Nearby creatures take damage and are knocked to the ground unless they pass a physical resistance check. They are also slowed briefly unless they pass another physical resistance check. After learning this talent, Shale gains a bonus to movement speed, while suffering a greater penalty to defense, whenever Pulverizing Blows is active.</t>
   </si>
   <si>
-    <t>1602176568</t>
-  </si>
-  <si>
     <t>Shale focuses strength into one devastating blow against an enemy. This attack gains bonus armor penetration and is an automatic critical hit if it connects. If the target has less than 50% health, this attack inflicts increasing damage as the target’s health diminishes. Shale suffers penalties to attack and stamina regeneration for a short time after using this attack. After learning this talent, Shale gains bonuses to damage, attack, armor penetration, and critical chance whenever Pulverizing Blows is active.</t>
   </si>
   <si>
-    <t>1602176569</t>
-  </si>
-  <si>
     <t>Shale activates a mode that focuses on defense, gaining bonuses to armor, physical, and elemental resistances, while suffering penalties to damage and critical chance. Whenever this mode is active, Shale’s threat toward all nearby enemies increases over time, making them more likely to target Shale. Bellow, Stone Will, and Regenerating Burst add bonuses to this mode.</t>
   </si>
   <si>
-    <t>1602176570</t>
-  </si>
-  <si>
     <t>Shale erupts with the sound of the Rock itself, stunning nearby enemies unless they pass a mental resistance check against Shale’s constitution. They are also dazed, and suffer penalties to attack and defense, unless they pass another mental resistance check against Shale’s constitution. Enemies stunned by this attack cannot resist being dazed. The power of this talent depends on Shale's constitution. This talent increases the bonuses of Stoneheart.</t>
   </si>
   <si>
-    <t>1602176571</t>
-  </si>
-  <si>
     <t>Shale attracts the attention of a single enemy, who now views Shale as the most urgent threat on the battlefield and is likely to target Shale. After this talent is learned, Stoneheart will also give Shale bonuses to health regeneration and stamina regeneration, and enemies are even more likely to target Shale when that mode is active.</t>
   </si>
   <si>
-    <t>1602176572</t>
-  </si>
-  <si>
     <t>Shale explodes with energy, damaging all nearby enemies. Enemies hit by the explosion are knocked down or knocked back unless they pass a physical resistance check against Shale’s constitution. They are also stunned unless they pass a mental resistance check against Shale’s constitution. The energy gives Shale a burst of health regeneration and stamina regeneration. The lower Shale's health or stamina, the stronger the regeneration. The power of this talent also depends on Shale's constitution. This talent further increases the bonuses of Stoneheart.</t>
   </si>
   <si>
-    <t>1602176573</t>
-  </si>
-  <si>
     <t>Shale activates a mode that enables long-range attacks, gaining a large defense bonus against missile attacks while suffering penalties to attack and movement speed. While in this mode, Shale emanates an aura that grants nearby party members bonuses to ranged critical chance and ranged attack speed. Hurl Rock, Earthen Grasp, and Rock Barrage add bonuses to this mode.</t>
   </si>
   <si>
-    <t>1602176574</t>
-  </si>
-  <si>
     <t>Shale pulls a rock from the ground and hurls it to a location, dealing physical damage to all creatures in the impact area. Creatures closer to the center of the impact take more damage, and those within 3 meters of the center are also knocked down unless they pass a physical resistance check against Shale's strength. Friendly fire possible. This talent increases the bonuses for party members and Shale’s missile deflection.</t>
   </si>
   <si>
-    <t>1602176575</t>
-  </si>
-  <si>
     <t>Shale pounds the earth, immobilizing enemies unless they pass a physical resistance check, in which case they suffer penalties to attack speed and movement speed instead. Shale’s willpower increases the duration of the effects. This talent further increases Shale’s missile deflection.</t>
   </si>
   <si>
-    <t>1602176576</t>
-  </si>
-  <si>
     <t>Shale tosses up multiple rocks that crash down in the targeted area. Creatures within the area take damage and are knocked down or knocked back unless they pass a physical resistance check. Friendly fire possible. This talent increases the bonuses for party members and Shale’s missile deflection. Nearby party members now also gain bonuses to attack and damage when using ranged weapons. Additionally, Shale’s aura can now shield others, granting party members within 3 meters a bonus to missile deflection.</t>
   </si>
   <si>
-    <t>1602176577</t>
-  </si>
-  <si>
     <t>Shale activates a support mode that imbues nearby party members with bonuses to defense, armor, and all resistances. Shale is immobilized when in this mode, suffering a penalty to defense while gaining bonuses to armor, physical, spell, and elemental resistances. Inner Reserves, Renewed Assault, and Supernatural Resilience add bonuses to this mode.</t>
   </si>
   <si>
-    <t>1602176578</t>
-  </si>
-  <si>
     <t>Whenever Stone Aura is active, party members within the aura now receive bonuses to health regeneration, stamina regeneration, and spellpower. This talent also increases the radius of Stone Aura.</t>
   </si>
   <si>
-    <t>1602176579</t>
-  </si>
-  <si>
     <t>Whenever Stone Aura is active, Shale gains additional bonuses to armor, spell, and elemental resistances. Party members within the aura gain additional bonuses to health regeneration, stamina regeneration, and spellpower, as well as a bonus to movement speed. This talent also increases the radius of Stone Aura.</t>
   </si>
   <si>
-    <t>1602176580</t>
-  </si>
-  <si>
     <t>Whenever Stone Aura is active, Shale gains additional bonuses to armor, physical, spell, and elemental resistances. Party members within the aura gain additional bonuses to defense, armor, and all resistances. The aura now also grants additional bonuses to party members when they stay close to Shale. This talent also increases the radius of Stone Aura.</t>
   </si>
   <si>
-    <t>1602176581</t>
-  </si>
-  <si>
     <t>Bonuses to damage and attack; penalties to defense and armor (Slam: bonus to armor penetration; Quake: bonus to movement speed).</t>
   </si>
   <si>
-    <t>1602176582</t>
-  </si>
-  <si>
     <t>Knocked down; possible penalty to movement speed.</t>
   </si>
   <si>
-    <t>1602176583</t>
-  </si>
-  <si>
     <t>Shale suffers reduced attack and stamina regeneration. Target is knocked down or knocked back.</t>
   </si>
   <si>
-    <t>1602176584</t>
-  </si>
-  <si>
     <t>Bonuses to armor, physical, and elemental resistances; penalties to damage and critical chance (Stone Will: bonus to health regeneration and stamina regeneration).</t>
   </si>
   <si>
-    <t>1602176585</t>
-  </si>
-  <si>
     <t>Stunned; possible penalties to attack and defense.</t>
   </si>
   <si>
-    <t>1602176586</t>
-  </si>
-  <si>
     <t>Shale gains increased health regeneration and stamina regeneration. Enemies are knocked down, knocked back, or stunned.</t>
   </si>
   <si>
-    <t>1602176587</t>
-  </si>
-  <si>
     <t>Shale gains increased missile deflection, but suffers reduced movement speed and attack. Party members gain bonuses to ranged critical chance and aim speed.</t>
   </si>
   <si>
-    <t>1602176588</t>
-  </si>
-  <si>
     <t>Paralyzed; penalties to attack speed and movement speed.</t>
   </si>
   <si>
-    <t>1602176589</t>
-  </si>
-  <si>
     <t>Knocked down or knocked back.</t>
   </si>
   <si>
-    <t>1602176590</t>
-  </si>
-  <si>
     <t>Shale is paralyzed but gains bonuses to armor and resistances. Party members gain bonuses to defense, armor, and resistances.</t>
   </si>
   <si>
-    <t>1602176591</t>
-  </si>
-  <si>
     <t>Bonuses to ranged attack and damage; possible bonus to missile deflection.</t>
   </si>
   <si>
-    <t>1602176592</t>
-  </si>
-  <si>
     <t>Bonuses to defense, armor, resistances, and spellpower.</t>
   </si>
   <si>
-    <t>1602176593</t>
-  </si>
-  <si>
     <t>Stone Will</t>
   </si>
   <si>
-    <t>1602176594</t>
-  </si>
-  <si>
     <t>With a will of stone, Shale becomes a living fortress. All active movement speed modifiers are immediately removed. For a time, Shale gains increased physical and mental resistances, and becomes immune to knockdown, knockback, and slip effects. All incoming damage is partially absorbed, until a maximum amount is reached. Shale is slowed during this time, but will also shrug off any incoming effect that would alter movement speed. The power of this talent depends on Shale's constitution. After this talent is learned, Shale gains bonuses to health regeneration and stamina regeneration whenever Stoneheart is active, and enemies are even more likely to target Shale.</t>
   </si>
   <si>
-    <t>1602176595</t>
-  </si>
-  <si>
     <t>Bonuses to physical and mental resistances; incoming damage is partially absorbed; immune to knockdown, knockback, slip, and movement speed modifications.</t>
   </si>
   <si>
-    <t>1602176596</t>
-  </si>
-  <si>
     <t>With a will of stone, Shale becomes a living fortress. All active movement speed modifiers are immediately removed. For a time, Shale gains increased physical and mental resistances, and becomes immune to knockdown, stun, and slip effects. All incoming damage is partially absorbed, until a maximum amount is reached. Shale is slowed during this time, but will also shrug off any incoming effect that would alter movement speed. The power of this talent depends on Shale's constitution. After this talent is learned, Shale gains bonuses to health regeneration and stamina regeneration whenever Stoneheart is active, and enemies are even more likely to target Shale.</t>
-  </si>
-  <si>
-    <t>1602176597</t>
   </si>
   <si>
     <t>Bonuses to physical and mental resistances; incoming damage is partially absorbed; immune to knockdown, stun, slip, and movement speed modifications.</t>
@@ -2803,6 +2704,105 @@
   </si>
   <si>
     <t>This spell allows you to channel more of your power into the lock, opening more complex varieties.</t>
+  </si>
+  <si>
+    <t>6610018</t>
+  </si>
+  <si>
+    <t>6610019</t>
+  </si>
+  <si>
+    <t>6610020</t>
+  </si>
+  <si>
+    <t>6610021</t>
+  </si>
+  <si>
+    <t>6610022</t>
+  </si>
+  <si>
+    <t>6610023</t>
+  </si>
+  <si>
+    <t>6610024</t>
+  </si>
+  <si>
+    <t>6610025</t>
+  </si>
+  <si>
+    <t>6610026</t>
+  </si>
+  <si>
+    <t>6610027</t>
+  </si>
+  <si>
+    <t>6610028</t>
+  </si>
+  <si>
+    <t>6610029</t>
+  </si>
+  <si>
+    <t>6610030</t>
+  </si>
+  <si>
+    <t>6610031</t>
+  </si>
+  <si>
+    <t>6610032</t>
+  </si>
+  <si>
+    <t>6610033</t>
+  </si>
+  <si>
+    <t>6610034</t>
+  </si>
+  <si>
+    <t>6610035</t>
+  </si>
+  <si>
+    <t>6610036</t>
+  </si>
+  <si>
+    <t>6610037</t>
+  </si>
+  <si>
+    <t>6610038</t>
+  </si>
+  <si>
+    <t>6610039</t>
+  </si>
+  <si>
+    <t>6610040</t>
+  </si>
+  <si>
+    <t>6610041</t>
+  </si>
+  <si>
+    <t>6610042</t>
+  </si>
+  <si>
+    <t>6610043</t>
+  </si>
+  <si>
+    <t>6610044</t>
+  </si>
+  <si>
+    <t>6610045</t>
+  </si>
+  <si>
+    <t>6610046</t>
+  </si>
+  <si>
+    <t>6610047</t>
+  </si>
+  <si>
+    <t>6610048</t>
+  </si>
+  <si>
+    <t>6610049</t>
+  </si>
+  <si>
+    <t>6610050</t>
   </si>
 </sst>
 </file>
@@ -3206,8 +3206,8 @@
   <dimension ref="A1:B473"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B446" sqref="B446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3246,7 +3246,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>865</v>
+        <v>832</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3259,31 +3259,31 @@
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>887</v>
+        <v>854</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>872</v>
+        <v>839</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>888</v>
+        <v>855</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>871</v>
+        <v>838</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>889</v>
+        <v>856</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>870</v>
+        <v>837</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>890</v>
+        <v>857</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>104</v>
@@ -3291,7 +3291,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>891</v>
+        <v>858</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>105</v>
@@ -3299,935 +3299,935 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>892</v>
+        <v>859</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>906</v>
+        <v>873</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>893</v>
+        <v>860</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>905</v>
+        <v>872</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>894</v>
+        <v>861</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>904</v>
+        <v>871</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>895</v>
+        <v>862</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>907</v>
+        <v>874</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>896</v>
+        <v>863</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>899</v>
+        <v>866</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>897</v>
+        <v>864</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>898</v>
+        <v>865</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>900</v>
+        <v>867</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>901</v>
+        <v>868</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>902</v>
+        <v>869</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>903</v>
+        <v>870</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>646</v>
+        <v>613</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>647</v>
+        <v>614</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>648</v>
+        <v>615</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>649</v>
+        <v>616</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>650</v>
+        <v>617</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>651</v>
+        <v>618</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>652</v>
+        <v>619</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>653</v>
+        <v>620</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>654</v>
+        <v>621</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>655</v>
+        <v>622</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>656</v>
+        <v>623</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>875</v>
+        <v>842</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>657</v>
+        <v>624</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>658</v>
+        <v>625</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>659</v>
+        <v>626</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>660</v>
+        <v>627</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>661</v>
+        <v>628</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>662</v>
+        <v>629</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>663</v>
+        <v>630</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>664</v>
+        <v>631</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>665</v>
+        <v>632</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>876</v>
+        <v>843</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>666</v>
+        <v>633</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>667</v>
+        <v>634</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>668</v>
+        <v>635</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>669</v>
+        <v>636</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>670</v>
+        <v>637</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>647</v>
+        <v>614</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>671</v>
+        <v>638</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>877</v>
+        <v>844</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>672</v>
+        <v>639</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>880</v>
+        <v>847</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>673</v>
+        <v>640</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>878</v>
+        <v>845</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>674</v>
+        <v>641</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>675</v>
+        <v>642</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>676</v>
+        <v>643</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>879</v>
+        <v>846</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>677</v>
+        <v>644</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>678</v>
+        <v>645</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>679</v>
+        <v>646</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>881</v>
+        <v>848</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>680</v>
+        <v>647</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>882</v>
+        <v>849</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>681</v>
+        <v>648</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>883</v>
+        <v>850</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>682</v>
+        <v>649</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>683</v>
+        <v>650</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>684</v>
+        <v>651</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>884</v>
+        <v>851</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>685</v>
+        <v>652</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>686</v>
+        <v>653</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>687</v>
+        <v>654</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>688</v>
+        <v>655</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>689</v>
+        <v>656</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>649</v>
+        <v>616</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>691</v>
+        <v>658</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>692</v>
+        <v>659</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>693</v>
+        <v>660</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>694</v>
+        <v>661</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>695</v>
+        <v>662</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>696</v>
+        <v>663</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>622</v>
+        <v>589</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>697</v>
+        <v>664</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>624</v>
+        <v>591</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>698</v>
+        <v>665</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>699</v>
+        <v>666</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>700</v>
+        <v>667</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>701</v>
+        <v>668</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>702</v>
+        <v>669</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>703</v>
+        <v>670</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>704</v>
+        <v>671</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>705</v>
+        <v>672</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>706</v>
+        <v>673</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>707</v>
+        <v>674</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>708</v>
+        <v>675</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>709</v>
+        <v>676</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>710</v>
+        <v>677</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>711</v>
+        <v>678</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>712</v>
+        <v>679</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>713</v>
+        <v>680</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>714</v>
+        <v>681</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>715</v>
+        <v>682</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>716</v>
+        <v>683</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>717</v>
+        <v>684</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>718</v>
+        <v>685</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>719</v>
+        <v>686</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>720</v>
+        <v>687</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>721</v>
+        <v>688</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>722</v>
+        <v>689</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>723</v>
+        <v>690</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>724</v>
+        <v>691</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>725</v>
+        <v>692</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>726</v>
+        <v>693</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>727</v>
+        <v>694</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>728</v>
+        <v>695</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>729</v>
+        <v>696</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>730</v>
+        <v>697</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>731</v>
+        <v>698</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>732</v>
+        <v>699</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>733</v>
+        <v>700</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>734</v>
+        <v>701</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>735</v>
+        <v>702</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>736</v>
+        <v>703</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>737</v>
+        <v>704</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>738</v>
+        <v>705</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>739</v>
+        <v>706</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>740</v>
+        <v>707</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>741</v>
+        <v>708</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>742</v>
+        <v>709</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>743</v>
+        <v>710</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>744</v>
+        <v>711</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>745</v>
+        <v>712</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>746</v>
+        <v>713</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>747</v>
+        <v>714</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>748</v>
+        <v>715</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>749</v>
+        <v>716</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>750</v>
+        <v>717</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>751</v>
+        <v>718</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>752</v>
+        <v>719</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>753</v>
+        <v>720</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>754</v>
+        <v>721</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>755</v>
+        <v>722</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>756</v>
+        <v>723</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>757</v>
+        <v>724</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>758</v>
+        <v>725</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>759</v>
+        <v>726</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>760</v>
+        <v>727</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>761</v>
+        <v>728</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>762</v>
+        <v>729</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>763</v>
+        <v>730</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>764</v>
+        <v>731</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>765</v>
+        <v>732</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>766</v>
+        <v>733</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>767</v>
+        <v>734</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>768</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>769</v>
+        <v>736</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>770</v>
+        <v>737</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>771</v>
+        <v>738</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>772</v>
+        <v>739</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>773</v>
+        <v>740</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>774</v>
+        <v>741</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>775</v>
+        <v>742</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>776</v>
+        <v>743</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>777</v>
+        <v>744</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>719</v>
+        <v>686</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>778</v>
+        <v>745</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>721</v>
+        <v>688</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>779</v>
+        <v>746</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>780</v>
+        <v>747</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>781</v>
+        <v>748</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>782</v>
+        <v>749</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>783</v>
+        <v>750</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>784</v>
+        <v>751</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>631</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>785</v>
+        <v>752</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>786</v>
+        <v>753</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>787</v>
+        <v>754</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>874</v>
+        <v>841</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>788</v>
+        <v>755</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>789</v>
+        <v>756</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>790</v>
+        <v>757</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>791</v>
+        <v>758</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>885</v>
+        <v>852</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>792</v>
+        <v>759</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>271</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>793</v>
+        <v>760</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>794</v>
+        <v>761</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>795</v>
+        <v>762</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>796</v>
+        <v>763</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>797</v>
+        <v>764</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>798</v>
+        <v>765</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>799</v>
+        <v>766</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>886</v>
+        <v>853</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>800</v>
+        <v>767</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>801</v>
+        <v>768</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>802</v>
+        <v>769</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>803</v>
+        <v>770</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>804</v>
+        <v>771</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>805</v>
+        <v>772</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>806</v>
+        <v>773</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>807</v>
+        <v>774</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>808</v>
+        <v>775</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>809</v>
+        <v>776</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>810</v>
+        <v>777</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>811</v>
+        <v>778</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>812</v>
+        <v>779</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>813</v>
+        <v>780</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>814</v>
+        <v>781</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>815</v>
+        <v>782</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>816</v>
+        <v>783</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>817</v>
+        <v>784</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>818</v>
+        <v>785</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>819</v>
+        <v>786</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>820</v>
+        <v>787</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>821</v>
+        <v>788</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>822</v>
+        <v>789</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>823</v>
+        <v>790</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>824</v>
+        <v>791</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>825</v>
+        <v>792</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>826</v>
+        <v>793</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>827</v>
+        <v>794</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>828</v>
+        <v>795</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>829</v>
+        <v>796</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>830</v>
+        <v>797</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>831</v>
+        <v>798</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>71</v>
@@ -4235,55 +4235,55 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>832</v>
+        <v>799</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>833</v>
+        <v>800</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>834</v>
+        <v>801</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>835</v>
+        <v>802</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>836</v>
+        <v>803</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>837</v>
+        <v>804</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>838</v>
+        <v>805</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>839</v>
+        <v>806</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>840</v>
+        <v>807</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>841</v>
+        <v>808</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>842</v>
+        <v>809</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>843</v>
+        <v>810</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>844</v>
+        <v>811</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>71</v>
@@ -4291,90 +4291,90 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>845</v>
+        <v>812</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>846</v>
+        <v>813</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>847</v>
+        <v>814</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>848</v>
+        <v>815</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>849</v>
+        <v>816</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>850</v>
+        <v>817</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>851</v>
+        <v>818</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>852</v>
+        <v>819</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>853</v>
+        <v>820</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>854</v>
+        <v>821</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>855</v>
+        <v>822</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>856</v>
+        <v>823</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>857</v>
+        <v>824</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>858</v>
+        <v>825</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>859</v>
+        <v>826</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>860</v>
+        <v>827</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>669</v>
+        <v>636</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>861</v>
+        <v>828</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>862</v>
+        <v>829</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>863</v>
+        <v>830</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>864</v>
+        <v>831</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -4483,1842 +4483,1842 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>243</v>
+        <v>210</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>261</v>
+        <v>228</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>264</v>
+        <v>231</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>268</v>
+        <v>235</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>270</v>
+        <v>237</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>271</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>272</v>
+        <v>239</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>274</v>
+        <v>241</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>275</v>
+        <v>242</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>276</v>
+        <v>243</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>279</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>280</v>
+        <v>247</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>281</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>283</v>
+        <v>250</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>285</v>
+        <v>252</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>286</v>
+        <v>253</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>289</v>
+        <v>256</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>290</v>
+        <v>257</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>291</v>
+        <v>258</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>292</v>
+        <v>259</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>294</v>
+        <v>261</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>295</v>
+        <v>262</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>296</v>
+        <v>263</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>297</v>
+        <v>264</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>298</v>
+        <v>265</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>299</v>
+        <v>266</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>301</v>
+        <v>268</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>302</v>
+        <v>269</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>303</v>
+        <v>270</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>305</v>
+        <v>272</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>308</v>
+        <v>275</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>310</v>
+        <v>277</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>311</v>
+        <v>278</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>318</v>
+        <v>285</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>319</v>
+        <v>286</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>320</v>
+        <v>287</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>321</v>
+        <v>288</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>322</v>
+        <v>289</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>323</v>
+        <v>290</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>324</v>
+        <v>291</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>325</v>
+        <v>292</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>326</v>
+        <v>293</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>327</v>
+        <v>294</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>328</v>
+        <v>295</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>329</v>
+        <v>296</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>330</v>
+        <v>297</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>331</v>
+        <v>298</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>332</v>
+        <v>299</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>334</v>
+        <v>301</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>335</v>
+        <v>302</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>336</v>
+        <v>303</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>337</v>
+        <v>304</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>338</v>
+        <v>305</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>339</v>
+        <v>306</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>340</v>
+        <v>307</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>341</v>
+        <v>308</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>343</v>
+        <v>310</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>344</v>
+        <v>311</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>345</v>
+        <v>312</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>346</v>
+        <v>313</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>347</v>
+        <v>314</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>348</v>
+        <v>315</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>349</v>
+        <v>316</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>350</v>
+        <v>317</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>351</v>
+        <v>318</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>352</v>
+        <v>319</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>353</v>
+        <v>320</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>354</v>
+        <v>321</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>355</v>
+        <v>322</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>356</v>
+        <v>323</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>357</v>
+        <v>324</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>358</v>
+        <v>325</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>359</v>
+        <v>326</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>360</v>
+        <v>327</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>361</v>
+        <v>328</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>362</v>
+        <v>329</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>363</v>
+        <v>330</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>364</v>
+        <v>331</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>365</v>
+        <v>332</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>366</v>
+        <v>333</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>367</v>
+        <v>334</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>368</v>
+        <v>335</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>369</v>
+        <v>336</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>370</v>
+        <v>337</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>371</v>
+        <v>338</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>372</v>
+        <v>339</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>373</v>
+        <v>340</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>374</v>
+        <v>341</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>375</v>
+        <v>342</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>376</v>
+        <v>343</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>377</v>
+        <v>344</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>379</v>
+        <v>346</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>380</v>
+        <v>347</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>381</v>
+        <v>348</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>382</v>
+        <v>349</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>383</v>
+        <v>350</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>384</v>
+        <v>351</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>385</v>
+        <v>352</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>387</v>
+        <v>354</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>388</v>
+        <v>355</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>389</v>
+        <v>356</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>390</v>
+        <v>357</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>391</v>
+        <v>358</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>392</v>
+        <v>359</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>393</v>
+        <v>360</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>394</v>
+        <v>361</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>395</v>
+        <v>362</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>397</v>
+        <v>364</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>398</v>
+        <v>365</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>400</v>
+        <v>367</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>401</v>
+        <v>368</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>402</v>
+        <v>369</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>403</v>
+        <v>370</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>404</v>
+        <v>371</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>405</v>
+        <v>372</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>406</v>
+        <v>373</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>408</v>
+        <v>375</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>409</v>
+        <v>376</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>410</v>
+        <v>377</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>411</v>
+        <v>378</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>412</v>
+        <v>379</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>413</v>
+        <v>380</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>414</v>
+        <v>381</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>415</v>
+        <v>382</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>416</v>
+        <v>383</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>417</v>
+        <v>384</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>418</v>
+        <v>385</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>419</v>
+        <v>386</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>420</v>
+        <v>387</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>421</v>
+        <v>388</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>422</v>
+        <v>389</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>423</v>
+        <v>390</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>424</v>
+        <v>391</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>425</v>
+        <v>392</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>426</v>
+        <v>393</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>428</v>
+        <v>395</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>429</v>
+        <v>396</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>430</v>
+        <v>397</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>431</v>
+        <v>398</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>432</v>
+        <v>399</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>433</v>
+        <v>400</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>434</v>
+        <v>401</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>435</v>
+        <v>402</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>438</v>
+        <v>405</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>439</v>
+        <v>406</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>441</v>
+        <v>408</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>442</v>
+        <v>409</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>443</v>
+        <v>410</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>444</v>
+        <v>411</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>445</v>
+        <v>412</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>446</v>
+        <v>413</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>447</v>
+        <v>414</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>448</v>
+        <v>415</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>449</v>
+        <v>416</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>450</v>
+        <v>417</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>451</v>
+        <v>418</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>452</v>
+        <v>419</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>453</v>
+        <v>420</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>454</v>
+        <v>421</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>455</v>
+        <v>422</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>456</v>
+        <v>423</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>457</v>
+        <v>424</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>458</v>
+        <v>425</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>459</v>
+        <v>426</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>460</v>
+        <v>427</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>461</v>
+        <v>428</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>462</v>
+        <v>429</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>463</v>
+        <v>430</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>464</v>
+        <v>431</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>465</v>
+        <v>432</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>466</v>
+        <v>433</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>467</v>
+        <v>434</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>468</v>
+        <v>435</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>470</v>
+        <v>437</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>471</v>
+        <v>438</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>472</v>
+        <v>439</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>473</v>
+        <v>440</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>474</v>
+        <v>441</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>476</v>
+        <v>443</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>479</v>
+        <v>446</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>480</v>
+        <v>447</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>481</v>
+        <v>448</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>482</v>
+        <v>449</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>483</v>
+        <v>450</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>484</v>
+        <v>451</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>485</v>
+        <v>452</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>486</v>
+        <v>453</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>487</v>
+        <v>454</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>488</v>
+        <v>455</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>489</v>
+        <v>456</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>490</v>
+        <v>457</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>491</v>
+        <v>458</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>493</v>
+        <v>460</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>494</v>
+        <v>461</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>495</v>
+        <v>462</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>496</v>
+        <v>463</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>497</v>
+        <v>464</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>498</v>
+        <v>465</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>499</v>
+        <v>466</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>500</v>
+        <v>467</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>501</v>
+        <v>468</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>502</v>
+        <v>469</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>503</v>
+        <v>470</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>504</v>
+        <v>471</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>505</v>
+        <v>472</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>506</v>
+        <v>473</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>507</v>
+        <v>474</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>508</v>
+        <v>475</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>509</v>
+        <v>476</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>510</v>
+        <v>477</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>511</v>
+        <v>478</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>512</v>
+        <v>479</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>513</v>
+        <v>480</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>514</v>
+        <v>481</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>515</v>
+        <v>482</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>516</v>
+        <v>483</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>517</v>
+        <v>484</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>518</v>
+        <v>485</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>519</v>
+        <v>486</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>520</v>
+        <v>487</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>521</v>
+        <v>488</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>522</v>
+        <v>489</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>523</v>
+        <v>490</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>524</v>
+        <v>491</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>525</v>
+        <v>492</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>526</v>
+        <v>493</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>527</v>
+        <v>494</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>528</v>
+        <v>495</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>529</v>
+        <v>496</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>530</v>
+        <v>497</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
-        <v>531</v>
+        <v>498</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>532</v>
+        <v>499</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
-        <v>533</v>
+        <v>500</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>534</v>
+        <v>501</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
-        <v>535</v>
+        <v>502</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
-        <v>537</v>
+        <v>504</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>538</v>
+        <v>505</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="s">
-        <v>539</v>
+        <v>506</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>540</v>
+        <v>507</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
-        <v>541</v>
+        <v>508</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>542</v>
+        <v>509</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
-        <v>543</v>
+        <v>510</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>544</v>
+        <v>511</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
-        <v>547</v>
+        <v>514</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>548</v>
+        <v>515</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
-        <v>549</v>
+        <v>516</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>550</v>
+        <v>517</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
-        <v>551</v>
+        <v>518</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>552</v>
+        <v>519</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
-        <v>553</v>
+        <v>520</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>554</v>
+        <v>521</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
-        <v>555</v>
+        <v>522</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>556</v>
+        <v>523</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
-        <v>557</v>
+        <v>524</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>558</v>
+        <v>525</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
-        <v>559</v>
+        <v>526</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>560</v>
+        <v>527</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
-        <v>561</v>
+        <v>528</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>562</v>
+        <v>529</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
-        <v>563</v>
+        <v>530</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>564</v>
+        <v>531</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
-        <v>565</v>
+        <v>532</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>566</v>
+        <v>533</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="s">
-        <v>567</v>
+        <v>534</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>568</v>
+        <v>535</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
-        <v>569</v>
+        <v>536</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>570</v>
+        <v>537</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
-        <v>571</v>
+        <v>538</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>572</v>
+        <v>539</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
-        <v>573</v>
+        <v>540</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>574</v>
+        <v>541</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
-        <v>575</v>
+        <v>542</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>576</v>
+        <v>543</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
-        <v>577</v>
+        <v>544</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>578</v>
+        <v>545</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
-        <v>579</v>
+        <v>546</v>
       </c>
       <c r="B336" s="4" t="s">
-        <v>580</v>
+        <v>547</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
-        <v>581</v>
+        <v>548</v>
       </c>
       <c r="B337" s="4" t="s">
-        <v>582</v>
+        <v>549</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
-        <v>583</v>
+        <v>550</v>
       </c>
       <c r="B338" s="4" t="s">
-        <v>584</v>
+        <v>551</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
-        <v>585</v>
+        <v>552</v>
       </c>
       <c r="B339" s="4" t="s">
-        <v>586</v>
+        <v>553</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
-        <v>587</v>
+        <v>554</v>
       </c>
       <c r="B340" s="4" t="s">
-        <v>588</v>
+        <v>555</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
-        <v>589</v>
+        <v>556</v>
       </c>
       <c r="B341" s="4" t="s">
-        <v>590</v>
+        <v>557</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
-        <v>591</v>
+        <v>558</v>
       </c>
       <c r="B342" s="4" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="B343" s="4" t="s">
-        <v>594</v>
+        <v>561</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
-        <v>595</v>
+        <v>562</v>
       </c>
       <c r="B344" s="4" t="s">
-        <v>596</v>
+        <v>563</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
-        <v>597</v>
+        <v>564</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>598</v>
+        <v>565</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
-        <v>599</v>
+        <v>566</v>
       </c>
       <c r="B346" s="4" t="s">
-        <v>600</v>
+        <v>567</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
-        <v>601</v>
+        <v>568</v>
       </c>
       <c r="B347" s="4" t="s">
-        <v>602</v>
+        <v>569</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="B348" s="4" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B349" s="4" t="s">
-        <v>606</v>
+        <v>573</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="s">
-        <v>607</v>
+        <v>574</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>608</v>
+        <v>575</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
-        <v>609</v>
+        <v>576</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>610</v>
+        <v>577</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
       <c r="B353" s="4" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="B354" s="4" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
-        <v>617</v>
+        <v>584</v>
       </c>
       <c r="B355" s="4" t="s">
-        <v>618</v>
+        <v>585</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="s">
-        <v>619</v>
+        <v>586</v>
       </c>
       <c r="B356" s="4" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
-        <v>621</v>
+        <v>588</v>
       </c>
       <c r="B357" s="4" t="s">
-        <v>622</v>
+        <v>589</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="s">
-        <v>623</v>
+        <v>590</v>
       </c>
       <c r="B358" s="4" t="s">
-        <v>624</v>
+        <v>591</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="B359" s="4" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="s">
-        <v>627</v>
+        <v>594</v>
       </c>
       <c r="B360" s="5" t="s">
-        <v>874</v>
+        <v>841</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="B361" s="4" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
       <c r="B362" s="4" t="s">
-        <v>631</v>
+        <v>598</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="s">
-        <v>632</v>
+        <v>599</v>
       </c>
       <c r="B363" s="4" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" s="3" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="B365" s="4" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
       <c r="B367" s="4" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
-        <v>642</v>
+        <v>609</v>
       </c>
       <c r="B368" s="4" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
-        <v>644</v>
+        <v>611</v>
       </c>
       <c r="B369" s="4" t="s">
-        <v>645</v>
+        <v>612</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="B371" s="4" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="B372" s="4" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="B373" s="4" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="3" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="B374" s="4" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="B376" s="4" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="B377" s="4" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
-        <v>216</v>
+        <v>183</v>
       </c>
       <c r="B379" s="4" t="s">
-        <v>217</v>
+        <v>184</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
-        <v>218</v>
+        <v>185</v>
       </c>
       <c r="B380" s="4" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="B381" s="4" t="s">
-        <v>221</v>
+        <v>188</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="B382" s="4" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
-        <v>224</v>
+        <v>191</v>
       </c>
       <c r="B383" s="4" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="B384" s="4" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="B385" s="4" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
       <c r="B386" s="4" t="s">
-        <v>873</v>
+        <v>840</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
-        <v>231</v>
+        <v>198</v>
       </c>
       <c r="B387" s="4" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
       <c r="B388" s="4" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
@@ -6342,7 +6342,7 @@
         <v>106</v>
       </c>
       <c r="B391" s="7" t="s">
-        <v>872</v>
+        <v>839</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
@@ -6358,7 +6358,7 @@
         <v>78</v>
       </c>
       <c r="B393" s="4" t="s">
-        <v>868</v>
+        <v>835</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
@@ -6390,7 +6390,7 @@
         <v>51</v>
       </c>
       <c r="B397" s="4" t="s">
-        <v>866</v>
+        <v>833</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
@@ -6566,7 +6566,7 @@
         <v>57</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>867</v>
+        <v>834</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="45" x14ac:dyDescent="0.2">
@@ -6574,7 +6574,7 @@
         <v>88</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>869</v>
+        <v>836</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
@@ -6739,266 +6739,266 @@
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="B441" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="B441" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A442" s="3" t="s">
-        <v>134</v>
+        <v>876</v>
       </c>
       <c r="B442" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
-        <v>136</v>
+        <v>877</v>
       </c>
       <c r="B443" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A444" s="3" t="s">
-        <v>138</v>
+        <v>878</v>
       </c>
       <c r="B444" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
-        <v>140</v>
+        <v>879</v>
       </c>
       <c r="B445" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
-        <v>142</v>
+        <v>880</v>
       </c>
       <c r="B446" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
-        <v>144</v>
+        <v>881</v>
       </c>
       <c r="B447" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
-        <v>146</v>
+        <v>882</v>
       </c>
       <c r="B448" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
-        <v>148</v>
+        <v>883</v>
       </c>
       <c r="B449" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A450" s="3" t="s">
-        <v>150</v>
+        <v>884</v>
       </c>
       <c r="B450" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" s="3" t="s">
-        <v>152</v>
+        <v>885</v>
       </c>
       <c r="B451" s="4" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A452" s="3" t="s">
-        <v>154</v>
+        <v>886</v>
       </c>
       <c r="B452" s="4" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A453" s="3" t="s">
-        <v>156</v>
+        <v>887</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" s="3" t="s">
-        <v>158</v>
+        <v>888</v>
       </c>
       <c r="B454" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A455" s="3" t="s">
-        <v>160</v>
+        <v>889</v>
       </c>
       <c r="B455" s="4" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A456" s="3" t="s">
-        <v>162</v>
+        <v>890</v>
       </c>
       <c r="B456" s="4" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" s="3" t="s">
-        <v>164</v>
+        <v>891</v>
       </c>
       <c r="B457" s="4" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" s="3" t="s">
-        <v>166</v>
+        <v>892</v>
       </c>
       <c r="B458" s="4" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" s="3" t="s">
-        <v>168</v>
+        <v>893</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" s="3" t="s">
-        <v>170</v>
+        <v>894</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" s="3" t="s">
-        <v>172</v>
+        <v>895</v>
       </c>
       <c r="B461" s="4" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" s="3" t="s">
-        <v>174</v>
+        <v>896</v>
       </c>
       <c r="B462" s="4" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" s="3" t="s">
-        <v>176</v>
+        <v>897</v>
       </c>
       <c r="B463" s="4" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" s="3" t="s">
-        <v>178</v>
+        <v>898</v>
       </c>
       <c r="B464" s="4" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="3" t="s">
-        <v>180</v>
+        <v>899</v>
       </c>
       <c r="B465" s="4" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="3" t="s">
-        <v>182</v>
+        <v>900</v>
       </c>
       <c r="B466" s="4" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" s="3" t="s">
-        <v>184</v>
+        <v>901</v>
       </c>
       <c r="B467" s="4" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" s="3" t="s">
-        <v>186</v>
+        <v>902</v>
       </c>
       <c r="B468" s="4" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" s="3" t="s">
-        <v>188</v>
+        <v>903</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A470" s="3" t="s">
-        <v>190</v>
+        <v>904</v>
       </c>
       <c r="B470" s="4" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" s="3" t="s">
-        <v>192</v>
+        <v>905</v>
       </c>
       <c r="B471" s="4" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A472" s="3" t="s">
-        <v>194</v>
+        <v>906</v>
       </c>
       <c r="B472" s="4" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" s="3" t="s">
-        <v>196</v>
+        <v>907</v>
       </c>
       <c r="B473" s="4" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge Extra Dog Slot mod
Merged in the mod as requires integration with the module event handler which cannot be done otherwise.
</commit_message>
<xml_diff>
--- a/source/strings.xlsx
+++ b/source/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid_mod\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE0F26-3EF4-4E59-B365-4C6818977C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BE78C1-B5A8-4F1D-A0D2-5E876A470CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="1350" windowWidth="18780" windowHeight="15645" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="31380" yWindow="2550" windowWidth="23880" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="924">
   <si>
     <t>C:/Users/Jim/Documents/BioWare/Dragon Age/addins/af_archid/module/override/</t>
   </si>
@@ -2803,6 +2803,72 @@
   </si>
   <si>
     <t>6610050</t>
+  </si>
+  <si>
+    <t>6610051</t>
+  </si>
+  <si>
+    <t>6610052</t>
+  </si>
+  <si>
+    <t>6610053</t>
+  </si>
+  <si>
+    <t>6610054</t>
+  </si>
+  <si>
+    <t>6610055</t>
+  </si>
+  <si>
+    <t>6610056</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a minor conflict with another mod.
+EVENT_TYPE_SUMMON_DIED is not getting routed to EDS. As a result, when summoned creatures die, the dog will not shift up to the uppermost summon slot. You will have to blow the whistle to re-summon the dog and shift the dog up manually.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a conflict with another mod that you have installed.
+EVENT_TYPE_DYING is not getting routed to EDS. As a result, when the owner of the dog dies, the dog will die as well and the portrait will disappear. If this happens, you will have to blow the whistle following combat to dismiss and then summon the dog.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a conflict with another mod that you have installed.
+EVENT_TYPE_PARTY_MEMBER_FIRED is not getting routed to EDS. As a result, you should make sure you blow the whistle and remove the dog BEFORE the game removes the party, or you may break the game.  Here is a known list of offending locations (you should probably write these down):
+Red Cliff:  When entering the fade to save the boy
+Circle OF Magi: When entering the fade because of the sloth demon on the 4th floor
+Orzamar : The provings.  Each round removes the party members
+Denerim : At the pearl. If you sleep with anyone, the party is removed.
+Denerim: If you win the lands meet and chose a 1 on 1 match with Logain.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a conflict with another mod that you have installed.
+EVENT_TYPE_DYING is not getting routed to EDS. As a result, when the owner of the dog dies, the dog will die as well and the portrait will disappear. If this happens, you will have to blow the whistle following combat to dismiss and then summon the dog.
+EVENT_TYPE_PARTY_MEMBER_FIRED is not getting routed to EDS. As a result, you should make sure you blow the whistle and remove the dog BEFORE the game removes the party, or you may break the game.  Here is a known list of offending locations (you should probably write these down):
+Red Cliff:  When entering the fade to save the boy
+Circle OF Magi: When entering the fade because of the sloth demon on the 4th floor
+Orzamar : The provings.  Each round removes the party members
+Denerim : At the pearl. If you sleep with anyone, the party is removed.
+Denerim: If you win the lands meet and chose a 1 on 1 match with Logain.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a minor conflict with another mod.
+EVENT_TYPE_COMMAND_PENDING or EVENT_TYPE_COMMAND_COMPLETE  is not getting routed to EDS. As a result, you should blow the whistle and remove the dog from the party before allowing Mages or Rogue-Rangers from summoning any creatures.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a minor conflict with another mod.
+EVENT_TYPE_SUMMON_DIED is not getting routed to EDS. As a result, when summoned creatures die, the dog will not shift up to the uppermost summon slot. You will have to blow the whistle to re-summon the dog and shift the dog up manually.
+EVENT_TYPE_COMMAND_PENDING or EVENT_TYPE_COMMAND_COMPLETE  is not getting routed to EDS. As a result, you should blow the whistle and remove the dog from the party before allowing Mages or Rogue-Rangers from summoning any creatures.</t>
+  </si>
+  <si>
+    <t>6610057</t>
+  </si>
+  <si>
+    <t>6610058</t>
+  </si>
+  <si>
+    <t>Dog Wistle</t>
+  </si>
+  <si>
+    <t>You found this whistle around the neck of your Mabari.</t>
   </si>
 </sst>
 </file>
@@ -2868,7 +2934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2885,6 +2951,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3203,17 +3270,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D158D-1FBF-4946-A52B-028752432AE5}">
-  <dimension ref="A1:B473"/>
+  <dimension ref="A1:B523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B446" sqref="B446"/>
+      <pane ySplit="1" topLeftCell="A473" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B484" sqref="B484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="209" style="4" customWidth="1"/>
+    <col min="2" max="2" width="164" style="4" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -6866,7 +6933,7 @@
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A457" s="3" t="s">
+      <c r="A457" s="8" t="s">
         <v>891</v>
       </c>
       <c r="B457" s="4" t="s">
@@ -6874,7 +6941,7 @@
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A458" s="3" t="s">
+      <c r="A458" s="8" t="s">
         <v>892</v>
       </c>
       <c r="B458" s="4" t="s">
@@ -6882,7 +6949,7 @@
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459" s="3" t="s">
+      <c r="A459" s="8" t="s">
         <v>893</v>
       </c>
       <c r="B459" s="4" t="s">
@@ -6890,7 +6957,7 @@
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A460" s="3" t="s">
+      <c r="A460" s="8" t="s">
         <v>894</v>
       </c>
       <c r="B460" s="4" t="s">
@@ -6898,7 +6965,7 @@
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A461" s="3" t="s">
+      <c r="A461" s="8" t="s">
         <v>895</v>
       </c>
       <c r="B461" s="4" t="s">
@@ -6906,7 +6973,7 @@
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A462" s="3" t="s">
+      <c r="A462" s="8" t="s">
         <v>896</v>
       </c>
       <c r="B462" s="4" t="s">
@@ -6914,7 +6981,7 @@
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A463" s="3" t="s">
+      <c r="A463" s="8" t="s">
         <v>897</v>
       </c>
       <c r="B463" s="4" t="s">
@@ -6922,7 +6989,7 @@
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A464" s="3" t="s">
+      <c r="A464" s="8" t="s">
         <v>898</v>
       </c>
       <c r="B464" s="4" t="s">
@@ -6930,7 +6997,7 @@
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A465" s="3" t="s">
+      <c r="A465" s="8" t="s">
         <v>899</v>
       </c>
       <c r="B465" s="4" t="s">
@@ -6938,7 +7005,7 @@
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A466" s="3" t="s">
+      <c r="A466" s="8" t="s">
         <v>900</v>
       </c>
       <c r="B466" s="4" t="s">
@@ -6946,7 +7013,7 @@
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A467" s="3" t="s">
+      <c r="A467" s="8" t="s">
         <v>901</v>
       </c>
       <c r="B467" s="4" t="s">
@@ -6954,7 +7021,7 @@
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A468" s="3" t="s">
+      <c r="A468" s="8" t="s">
         <v>902</v>
       </c>
       <c r="B468" s="4" t="s">
@@ -6962,7 +7029,7 @@
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A469" s="3" t="s">
+      <c r="A469" s="8" t="s">
         <v>903</v>
       </c>
       <c r="B469" s="4" t="s">
@@ -6970,7 +7037,7 @@
       </c>
     </row>
     <row r="470" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A470" s="3" t="s">
+      <c r="A470" s="8" t="s">
         <v>904</v>
       </c>
       <c r="B470" s="4" t="s">
@@ -6978,7 +7045,7 @@
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A471" s="3" t="s">
+      <c r="A471" s="8" t="s">
         <v>905</v>
       </c>
       <c r="B471" s="4" t="s">
@@ -6986,7 +7053,7 @@
       </c>
     </row>
     <row r="472" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A472" s="3" t="s">
+      <c r="A472" s="8" t="s">
         <v>906</v>
       </c>
       <c r="B472" s="4" t="s">
@@ -6994,12 +7061,202 @@
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A473" s="3" t="s">
+      <c r="A473" s="8" t="s">
         <v>907</v>
       </c>
       <c r="B473" s="4" t="s">
         <v>164</v>
       </c>
+    </row>
+    <row r="474" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A474" s="8" t="s">
+        <v>908</v>
+      </c>
+      <c r="B474" s="4" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A475" s="8" t="s">
+        <v>909</v>
+      </c>
+      <c r="B475" s="4" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A476" s="8" t="s">
+        <v>910</v>
+      </c>
+      <c r="B476" s="4" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A477" s="8" t="s">
+        <v>911</v>
+      </c>
+      <c r="B477" s="4" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A478" s="8" t="s">
+        <v>912</v>
+      </c>
+      <c r="B478" s="4" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A479" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="B479" s="4" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A480" s="8" t="s">
+        <v>920</v>
+      </c>
+      <c r="B480" s="4" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A481" s="8" t="s">
+        <v>921</v>
+      </c>
+      <c r="B481" s="4" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A482" s="8"/>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A483" s="8"/>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A484" s="8"/>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A485" s="8"/>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A486" s="8"/>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A487" s="8"/>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A488" s="8"/>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A489" s="8"/>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A490" s="8"/>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A491" s="8"/>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A492" s="8"/>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A493" s="8"/>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A494" s="8"/>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A495" s="8"/>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A496" s="8"/>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A497" s="8"/>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A498" s="8"/>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A499" s="8"/>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A500" s="8"/>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A501" s="8"/>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A502" s="8"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A503" s="8"/>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A504" s="8"/>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A505" s="8"/>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A506" s="8"/>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A507" s="8"/>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A508" s="8"/>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A509" s="8"/>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A510" s="8"/>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A511" s="8"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A512" s="8"/>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A513" s="8"/>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A514" s="8"/>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A515" s="8"/>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A516" s="8"/>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A517" s="8"/>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A518" s="8"/>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A519" s="8"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A520" s="8"/>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A521" s="8"/>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A522" s="8"/>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A523" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B473">
@@ -7007,5 +7264,8 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A474:A477 A478:A481" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix broken spellshaping string references
The Spellshaping component string references were missing from the string table and had been reused by another component. This commit adds the strings back into the correct range and updates the references.
</commit_message>
<xml_diff>
--- a/source/strings.xlsx
+++ b/source/strings.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid_mod\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41051DE2-F745-4121-BE12-2D9C2F9A8E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99098805-896C-4A80-95DB-CDD516E390E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32130" yWindow="2070" windowWidth="21435" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="30780" yWindow="1095" windowWidth="21435" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$469</definedName>
+    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$465</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="876">
   <si>
     <t>C:/Users/Jim/Documents/BioWare/Dragon Age/addins/af_archid/module/override/</t>
   </si>
@@ -250,76 +250,28 @@
     <t>A short burst of arcane magic will deal with most simple locks.</t>
   </si>
   <si>
-    <t>627214948</t>
-  </si>
-  <si>
     <t>Friendly fire damage protection is extended to all allies on the battlefield.</t>
   </si>
   <si>
-    <t>627214943</t>
-  </si>
-  <si>
     <t>Spell Shaping</t>
   </si>
   <si>
-    <t>627214946</t>
-  </si>
-  <si>
     <t>Party members gain protection from the secondary effects of friendly spells such as knockdown, freezing and slow movement rate.</t>
   </si>
   <si>
-    <t>627214949</t>
-  </si>
-  <si>
     <t>Master Spell Shaping</t>
   </si>
   <si>
-    <t>627214951</t>
-  </si>
-  <si>
     <t>Warning: Spell Shaping Mod has detected a compatibility issue with one of the mods you have installed. Spell Shaping may not work properly.</t>
   </si>
   <si>
-    <t>627214952</t>
-  </si>
-  <si>
-    <t>Spell Shaping is a new skill mages can invest in to avoid friendly fire.</t>
-  </si>
-  <si>
-    <t>627214953</t>
-  </si>
-  <si>
-    <t>627214945</t>
-  </si>
-  <si>
     <t>Improved Spell Shaping</t>
   </si>
   <si>
-    <t>627214947</t>
-  </si>
-  <si>
     <t>Expert Spell Shaping</t>
   </si>
   <si>
-    <t>627214950</t>
-  </si>
-  <si>
     <t>Allies and party members no longer experience any damage or secondary effects from friendly wide-area spells.</t>
-  </si>
-  <si>
-    <t>627214954</t>
-  </si>
-  <si>
-    <t>Dheuster@gmail.com</t>
-  </si>
-  <si>
-    <t>627214955</t>
-  </si>
-  <si>
-    <t>http://social.bioware.com/project/1470/</t>
-  </si>
-  <si>
-    <t>627214944</t>
   </si>
   <si>
     <t>When active, the caster will shape and direct wide-area spells to avoid friendly fire at a cost of additional mana. Party members gain protection from the damage, with the additional mana spent based on the number of allies in the target area.</t>
@@ -3178,11 +3130,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D158D-1FBF-4946-A52B-028752432AE5}">
-  <dimension ref="A1:B477"/>
+  <dimension ref="A1:B473"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3221,7 +3173,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>794</v>
+        <v>778</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3234,31 +3186,31 @@
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>815</v>
+        <v>799</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>800</v>
+        <v>784</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>816</v>
+        <v>800</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>799</v>
+        <v>783</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>817</v>
+        <v>801</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>798</v>
+        <v>782</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>818</v>
+        <v>802</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>67</v>
@@ -3266,7 +3218,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>819</v>
+        <v>803</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>68</v>
@@ -3274,394 +3226,394 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>820</v>
+        <v>804</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>834</v>
+        <v>818</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>821</v>
+        <v>805</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>833</v>
+        <v>817</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>822</v>
+        <v>806</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>832</v>
+        <v>816</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>823</v>
+        <v>807</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>835</v>
+        <v>819</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>824</v>
+        <v>808</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>827</v>
+        <v>811</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>825</v>
+        <v>809</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>826</v>
+        <v>810</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>828</v>
+        <v>812</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>829</v>
+        <v>813</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>830</v>
+        <v>814</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>831</v>
+        <v>815</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>836</v>
+        <v>820</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>837</v>
+        <v>821</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>838</v>
+        <v>822</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>839</v>
+        <v>823</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>840</v>
+        <v>824</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>841</v>
+        <v>825</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>842</v>
+        <v>826</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>843</v>
+        <v>827</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>844</v>
+        <v>828</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>845</v>
+        <v>829</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>846</v>
+        <v>830</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>847</v>
+        <v>831</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>848</v>
+        <v>832</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>849</v>
+        <v>833</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>850</v>
+        <v>834</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>851</v>
+        <v>835</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>852</v>
+        <v>836</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>853</v>
+        <v>837</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>855</v>
+        <v>839</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>856</v>
+        <v>840</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>857</v>
+        <v>841</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>858</v>
+        <v>842</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>859</v>
+        <v>843</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>860</v>
+        <v>844</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>861</v>
+        <v>845</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>862</v>
+        <v>846</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>863</v>
+        <v>847</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>864</v>
+        <v>848</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>865</v>
+        <v>849</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>866</v>
+        <v>850</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>867</v>
+        <v>851</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>868</v>
+        <v>852</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>869</v>
+        <v>853</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>875</v>
+        <v>859</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>870</v>
+        <v>854</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>876</v>
+        <v>860</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>871</v>
+        <v>855</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>877</v>
+        <v>861</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>872</v>
+        <v>856</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>878</v>
+        <v>862</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>873</v>
+        <v>857</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>879</v>
+        <v>863</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>874</v>
+        <v>858</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>880</v>
+        <v>864</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>881</v>
+        <v>865</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>883</v>
+        <v>867</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>882</v>
+        <v>866</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>884</v>
+        <v>868</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -3677,7 +3629,7 @@
         <v>6610060</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>891</v>
+        <v>875</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -3797,7 +3749,7 @@
         <v>6610075</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>795</v>
+        <v>779</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -3821,7 +3773,7 @@
         <v>6610078</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>885</v>
+        <v>869</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -3829,7 +3781,7 @@
         <v>6610079</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>886</v>
+        <v>870</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -3837,7 +3789,7 @@
         <v>6610080</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>887</v>
+        <v>871</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -3845,7 +3797,7 @@
         <v>6610081</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>888</v>
+        <v>872</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -3853,7 +3805,7 @@
         <v>6610082</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>889</v>
+        <v>873</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -3861,7 +3813,7 @@
         <v>6610083</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>890</v>
+        <v>874</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="45" x14ac:dyDescent="0.2">
@@ -3869,7 +3821,7 @@
         <v>6610084</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>797</v>
+        <v>781</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
@@ -3877,7 +3829,7 @@
         <v>6610085</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>796</v>
+        <v>780</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -3889,3128 +3841,3096 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>575</v>
+      <c r="A88" s="9">
+        <v>6610087</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>577</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A89" s="9">
+        <v>6610088</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>578</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>579</v>
+      <c r="A90" s="9">
+        <v>6610089</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>580</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>581</v>
+      <c r="A91" s="9">
+        <v>6610090</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>582</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>583</v>
+      <c r="A92" s="9">
+        <v>6610091</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>585</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="9">
+        <v>6610092</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>803</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>586</v>
+      <c r="A94" s="9">
+        <v>6610093</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>587</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>588</v>
+      <c r="A95" s="9">
+        <v>6610094</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>589</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>590</v>
+      <c r="A96" s="9">
+        <v>6610095</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>591</v>
+        <v>73</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>594</v>
+        <v>561</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>804</v>
+        <v>562</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>595</v>
+        <v>563</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>596</v>
+        <v>564</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>597</v>
+        <v>565</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>598</v>
+        <v>566</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>599</v>
+        <v>567</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>600</v>
+        <v>569</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>601</v>
+        <v>570</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>602</v>
+        <v>572</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>806</v>
+        <v>573</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>603</v>
+        <v>574</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>606</v>
+        <v>578</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>609</v>
+        <v>581</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>610</v>
+        <v>583</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>611</v>
+        <v>584</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>612</v>
+        <v>789</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>613</v>
+        <v>585</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>614</v>
+        <v>586</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>615</v>
+        <v>790</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>616</v>
+        <v>587</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>618</v>
+        <v>589</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>578</v>
+        <v>791</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>619</v>
+        <v>590</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>621</v>
+        <v>592</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>623</v>
+        <v>593</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>625</v>
+        <v>594</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>551</v>
+        <v>795</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>626</v>
+        <v>595</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>627</v>
+        <v>597</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>185</v>
+        <v>796</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>628</v>
+        <v>598</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>187</v>
+        <v>599</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>629</v>
+        <v>600</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>630</v>
+        <v>601</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>631</v>
+        <v>602</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>632</v>
+        <v>562</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>633</v>
+        <v>603</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>634</v>
+        <v>604</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>635</v>
+        <v>605</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>636</v>
+        <v>606</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>637</v>
+        <v>607</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>638</v>
+        <v>608</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>639</v>
+        <v>609</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>640</v>
+        <v>535</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>641</v>
+        <v>610</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>642</v>
+        <v>537</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>643</v>
+        <v>611</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>644</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>645</v>
+        <v>612</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>646</v>
+        <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>647</v>
+        <v>613</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>648</v>
+        <v>614</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>649</v>
+        <v>615</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>650</v>
+        <v>616</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>651</v>
+        <v>617</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>652</v>
+        <v>618</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>653</v>
+        <v>619</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>654</v>
+        <v>620</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>655</v>
+        <v>621</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>656</v>
+        <v>622</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>657</v>
+        <v>623</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>658</v>
+        <v>624</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>659</v>
+        <v>625</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>660</v>
+        <v>626</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>661</v>
+        <v>627</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>662</v>
+        <v>628</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>663</v>
+        <v>629</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>664</v>
+        <v>630</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>665</v>
+        <v>631</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>666</v>
+        <v>632</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>667</v>
+        <v>633</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>669</v>
+        <v>635</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>671</v>
+        <v>637</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>672</v>
+        <v>638</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>673</v>
+        <v>639</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>674</v>
+        <v>640</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>675</v>
+        <v>641</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>676</v>
+        <v>642</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>677</v>
+        <v>643</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>678</v>
+        <v>644</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>679</v>
+        <v>645</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>680</v>
+        <v>646</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>681</v>
+        <v>647</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>682</v>
+        <v>648</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>683</v>
+        <v>649</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>196</v>
+        <v>650</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>684</v>
+        <v>651</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>198</v>
+        <v>652</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>685</v>
+        <v>653</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>686</v>
+        <v>654</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>687</v>
+        <v>655</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>202</v>
+        <v>658</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>690</v>
+        <v>659</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>691</v>
+        <v>660</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>692</v>
+        <v>661</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>693</v>
+        <v>662</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>694</v>
+        <v>663</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>695</v>
+        <v>664</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>696</v>
+        <v>665</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>697</v>
+        <v>666</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>698</v>
+        <v>667</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>699</v>
+        <v>180</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>700</v>
+        <v>668</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>701</v>
+        <v>182</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>702</v>
+        <v>669</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>206</v>
+        <v>670</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>703</v>
+        <v>671</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>206</v>
+        <v>672</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>704</v>
+        <v>673</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>705</v>
+        <v>186</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>706</v>
+        <v>674</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>648</v>
+        <v>675</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>707</v>
+        <v>676</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>708</v>
+        <v>678</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>709</v>
+        <v>679</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>710</v>
+        <v>680</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>545</v>
+        <v>681</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>711</v>
+        <v>682</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>712</v>
+        <v>683</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>713</v>
+        <v>684</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>560</v>
+        <v>685</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>714</v>
+        <v>686</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="B171" s="5" t="s">
-        <v>802</v>
+        <v>687</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>717</v>
+        <v>688</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>718</v>
+        <v>689</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>719</v>
+        <v>690</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>720</v>
+        <v>691</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>813</v>
+        <v>634</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>721</v>
+        <v>692</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>200</v>
+        <v>693</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>722</v>
+        <v>694</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>723</v>
+        <v>529</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>724</v>
+        <v>695</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>725</v>
+        <v>696</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>726</v>
+        <v>697</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>728</v>
+        <v>698</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>729</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>206</v>
+        <v>700</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>786</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>730</v>
+        <v>701</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>731</v>
+        <v>702</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>732</v>
+        <v>703</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>734</v>
+        <v>704</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>735</v>
+        <v>797</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>736</v>
+        <v>705</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>737</v>
+        <v>184</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>738</v>
+        <v>706</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>739</v>
+        <v>707</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>740</v>
+        <v>708</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>741</v>
+        <v>709</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>742</v>
+        <v>710</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>744</v>
+        <v>712</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>745</v>
+        <v>798</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>746</v>
+        <v>713</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>747</v>
+        <v>190</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>748</v>
+        <v>714</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>749</v>
+        <v>715</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>750</v>
+        <v>716</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>751</v>
+        <v>717</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>752</v>
+        <v>718</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>753</v>
+        <v>719</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>754</v>
+        <v>720</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>755</v>
+        <v>721</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>756</v>
+        <v>722</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>757</v>
+        <v>723</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>758</v>
+        <v>724</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>759</v>
+        <v>725</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>760</v>
+        <v>726</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>57</v>
+        <v>727</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>761</v>
+        <v>728</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>762</v>
+        <v>729</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>763</v>
+        <v>730</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>764</v>
+        <v>731</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>765</v>
+        <v>732</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>766</v>
+        <v>733</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>767</v>
+        <v>734</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>768</v>
+        <v>735</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>769</v>
+        <v>736</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>770</v>
+        <v>737</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>771</v>
+        <v>738</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>772</v>
+        <v>739</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>773</v>
+        <v>740</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>57</v>
+        <v>741</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>774</v>
+        <v>742</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>202</v>
+        <v>743</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>775</v>
+        <v>744</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>776</v>
+        <v>57</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>777</v>
+        <v>745</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>778</v>
+        <v>746</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>779</v>
+        <v>747</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>780</v>
+        <v>748</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>781</v>
+        <v>749</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>782</v>
+        <v>750</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>783</v>
+        <v>751</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>784</v>
+        <v>752</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>785</v>
+        <v>753</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>786</v>
+        <v>754</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>787</v>
+        <v>755</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>788</v>
+        <v>756</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>789</v>
+        <v>757</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>598</v>
+        <v>57</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>790</v>
+        <v>758</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>791</v>
+        <v>186</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>792</v>
+        <v>759</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>793</v>
+        <v>760</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>71</v>
+        <v>761</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>92</v>
+        <v>763</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>93</v>
+        <v>764</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>82</v>
+        <v>765</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>83</v>
+        <v>766</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>73</v>
+        <v>767</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>74</v>
+        <v>768</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>84</v>
+        <v>769</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>85</v>
+        <v>770</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>69</v>
+        <v>771</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>70</v>
+        <v>772</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>75</v>
+        <v>773</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>76</v>
+        <v>582</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>86</v>
+        <v>774</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>87</v>
+        <v>775</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>77</v>
+        <v>776</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>78</v>
+        <v>777</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>214</v>
+        <v>161</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B336" s="4" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B337" s="4" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B338" s="4" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="B339" s="4" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B340" s="4" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="B341" s="4" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B342" s="4" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B343" s="4" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="B344" s="4" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B346" s="4" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B347" s="4" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B348" s="4" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B349" s="4" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B353" s="4" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B354" s="4" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B355" s="4" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B356" s="4" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B357" s="4" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B358" s="4" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B359" s="4" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B360" s="4" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B361" s="4" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B362" s="4" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B363" s="4" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" s="3" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B365" s="4" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B367" s="4" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B368" s="4" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="B369" s="4" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B371" s="4" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B372" s="4" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B373" s="4" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="3" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B374" s="4" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B376" s="4" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B377" s="4" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B379" s="4" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B380" s="4" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="B381" s="4" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B382" s="4" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B383" s="4" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B384" s="4" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B385" s="4" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B386" s="4" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B387" s="4" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B388" s="4" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B389" s="4" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B390" s="4" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B391" s="4" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B392" s="4" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B393" s="4" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" s="3" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B394" s="4" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B395" s="4" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" s="3" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B396" s="4" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B397" s="4" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" s="3" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B398" s="4" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" s="3" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B399" s="4" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" s="3" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B401" s="4" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" s="3" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" s="3" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="B403" s="4" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" s="3" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="B404" s="4" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="B405" s="4" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" s="3" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B406" s="4" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" s="3" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="B407" s="4" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" s="3" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B408" s="4" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="B409" s="4" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" s="3" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="B410" s="4" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="B411" s="4" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" s="3" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B412" s="4" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" s="3" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" s="3" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B415" s="4" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" s="3" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="B416" s="4" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" s="3" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="B417" s="4" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" s="3" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B418" s="4" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" s="3" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="3" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" s="3" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" s="3" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="B422" s="4" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" s="3" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="B423" s="4" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" s="3" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="B424" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A425" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="B425" s="4" t="s">
-        <v>549</v>
+        <v>540</v>
+      </c>
+      <c r="B425" s="5" t="s">
+        <v>786</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" s="3" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="B426" s="4" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" s="3" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="B427" s="4" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" s="3" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="B428" s="4" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="429" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="B429" s="5" t="s">
-        <v>802</v>
+        <v>547</v>
+      </c>
+      <c r="B429" s="4" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" s="3" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="B430" s="4" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" s="3" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="B431" s="4" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" s="3" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="B432" s="4" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" s="3" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="B433" s="4" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A434" s="3" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="B434" s="4" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
-        <v>567</v>
+        <v>111</v>
       </c>
       <c r="B435" s="4" t="s">
-        <v>568</v>
+        <v>112</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
-        <v>569</v>
+        <v>113</v>
       </c>
       <c r="B436" s="4" t="s">
-        <v>570</v>
+        <v>114</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
-        <v>571</v>
+        <v>115</v>
       </c>
       <c r="B437" s="4" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="438" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" s="3" t="s">
-        <v>573</v>
+        <v>117</v>
       </c>
       <c r="B438" s="4" t="s">
-        <v>574</v>
+        <v>118</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B439" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B440" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B441" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B442" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B443" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B444" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B445" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B446" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B447" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B448" s="4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B449" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B450" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A451" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B451" s="4" t="s">
-        <v>152</v>
+        <v>785</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B452" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" s="3" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="B454" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" s="3" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="B455" s="4" t="s">
-        <v>801</v>
+        <v>46</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" s="3" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="B456" s="4" t="s">
-        <v>161</v>
+        <v>24</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" s="3" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="B457" s="4" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" s="3" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B458" s="4" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" s="3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B461" s="4" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B462" s="4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B463" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B464" s="4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B465" s="4" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B466" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B467" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B468" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B470" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B471" s="4" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" s="3" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B472" s="4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" s="3" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B473" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A474" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B474" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A475" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B475" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A476" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B476" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A477" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B477" s="4" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B477">
-    <sortCondition ref="A2:A477"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B473">
+    <sortCondition ref="A2:A473"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Extended Dog Talents mod
Merged in the mod abilities. There is no source code provided so compiled code included.
URL: https://www.nexusmods.com/dragonage/mods/1361
</commit_message>
<xml_diff>
--- a/source/strings.xlsx
+++ b/source/strings.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid_mod\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99098805-896C-4A80-95DB-CDD516E390E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C5CA6-3227-4C82-A3B8-5EFDBDB70ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30780" yWindow="1095" windowWidth="21435" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="2880" yWindow="1305" windowWidth="24090" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$465</definedName>
+    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$473</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="884">
   <si>
     <t>C:/Users/Jim/Documents/BioWare/Dragon Age/addins/af_archid/module/override/</t>
   </si>
@@ -2724,6 +2724,31 @@
   </si>
   <si>
     <t>There is a vial tied to the birds leg… &lt;act&gt;Try to take it!&lt;/act&gt;</t>
+  </si>
+  <si>
+    <t>Endurance</t>
+  </si>
+  <si>
+    <t>The mabari has undergone endurance and survival training, gaining a bonus to stamina.</t>
+  </si>
+  <si>
+    <t>Bond</t>
+  </si>
+  <si>
+    <t>Frighten</t>
+  </si>
+  <si>
+    <t>Ferocious bite</t>
+  </si>
+  <si>
+    <t>The mabari has formed a special bond with its master, gaining a bonus to mental resistance.</t>
+  </si>
+  <si>
+    <t>The mabari lets out a frightening howl, forcing nearby enemies to cower in fear unless they pass a mental resistance check.</t>
+  </si>
+  <si>
+    <t>The mabari will jump on its target and bite its neck. If the target is a living creature, it will die instantly if of normal or lesser rank unless it passes a physical resistance check. Lieutenant-ranked enemies will suffer a critical hit, while boss-ranked enemies will take only standard damage. Additionally, all targets who can bleed will take additional damage over time.
+Non-bleeding creatures will only take normal damage.</t>
   </si>
 </sst>
 </file>
@@ -3130,11 +3155,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D158D-1FBF-4946-A52B-028752432AE5}">
-  <dimension ref="A1:B473"/>
+  <dimension ref="A1:B481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3913,3024 +3938,3088 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>559</v>
+      <c r="A97" s="6">
+        <v>6610096</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>560</v>
+        <v>876</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
-        <v>561</v>
+      <c r="A98" s="6">
+        <v>6610097</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>562</v>
+        <v>877</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>563</v>
+      <c r="A99" s="6">
+        <v>6610098</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>564</v>
+        <v>878</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>565</v>
+      <c r="A100" s="6">
+        <v>6610099</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>566</v>
+        <v>881</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>567</v>
+      <c r="A101" s="6">
+        <v>6610100</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>569</v>
+        <v>879</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
+        <v>6610101</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>787</v>
+        <v>882</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>570</v>
+      <c r="A103" s="6">
+        <v>6610102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>572</v>
+        <v>880</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A104" s="6">
+        <v>6610103</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>573</v>
+        <v>883</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>788</v>
+        <v>564</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>790</v>
+        <v>575</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>794</v>
+        <v>560</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>596</v>
+        <v>792</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>601</v>
+        <v>791</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>608</v>
+        <v>795</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>537</v>
+        <v>796</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>169</v>
+        <v>599</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>171</v>
+        <v>601</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>614</v>
+        <v>562</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>622</v>
+        <v>535</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>624</v>
+        <v>537</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>626</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>628</v>
+        <v>171</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>629</v>
+        <v>613</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>630</v>
+        <v>614</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>631</v>
+        <v>615</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>632</v>
+        <v>616</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>634</v>
+        <v>618</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>635</v>
+        <v>619</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>636</v>
+        <v>620</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>638</v>
+        <v>622</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>639</v>
+        <v>623</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>641</v>
+        <v>625</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>642</v>
+        <v>626</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>644</v>
+        <v>628</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>645</v>
+        <v>629</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>646</v>
+        <v>630</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>648</v>
+        <v>632</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>651</v>
+        <v>635</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>652</v>
+        <v>636</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>654</v>
+        <v>638</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>655</v>
+        <v>639</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>656</v>
+        <v>640</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>658</v>
+        <v>642</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>659</v>
+        <v>643</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>660</v>
+        <v>644</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>661</v>
+        <v>645</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>665</v>
+        <v>649</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>666</v>
+        <v>650</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>667</v>
+        <v>651</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>180</v>
+        <v>652</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>182</v>
+        <v>654</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>186</v>
+        <v>660</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>681</v>
+        <v>180</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>682</v>
+        <v>668</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>683</v>
+        <v>182</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>684</v>
+        <v>669</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>190</v>
+        <v>672</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>632</v>
+        <v>677</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>634</v>
+        <v>679</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>692</v>
+        <v>680</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>693</v>
+        <v>681</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>694</v>
+        <v>682</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>529</v>
+        <v>683</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>695</v>
+        <v>684</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>696</v>
+        <v>685</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>544</v>
+        <v>190</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>786</v>
+        <v>688</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>701</v>
+        <v>690</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>702</v>
+        <v>632</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>703</v>
+        <v>691</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>704</v>
+        <v>692</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>797</v>
+        <v>693</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>184</v>
+        <v>529</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>709</v>
+        <v>544</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>710</v>
+        <v>698</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>712</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>798</v>
+        <v>700</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>786</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>713</v>
+        <v>701</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>190</v>
+        <v>702</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>716</v>
+        <v>704</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>717</v>
+        <v>797</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>719</v>
+        <v>184</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>727</v>
+        <v>798</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>728</v>
+        <v>713</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>729</v>
+        <v>190</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>731</v>
+        <v>715</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>732</v>
+        <v>716</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>734</v>
+        <v>718</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>736</v>
+        <v>720</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>741</v>
+        <v>725</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>744</v>
+        <v>728</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>57</v>
+        <v>729</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>745</v>
+        <v>730</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>746</v>
+        <v>731</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>747</v>
+        <v>732</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>748</v>
+        <v>733</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>749</v>
+        <v>734</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>751</v>
+        <v>736</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>753</v>
+        <v>738</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>754</v>
+        <v>739</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>755</v>
+        <v>740</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>57</v>
+        <v>743</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>186</v>
+        <v>57</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>768</v>
+        <v>754</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>772</v>
+        <v>57</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>582</v>
+        <v>186</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>775</v>
+        <v>760</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>148</v>
+        <v>763</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>149</v>
+        <v>764</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>150</v>
+        <v>765</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>151</v>
+        <v>766</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>152</v>
+        <v>767</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>153</v>
+        <v>768</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>154</v>
+        <v>769</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>155</v>
+        <v>770</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>156</v>
+        <v>771</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>157</v>
+        <v>772</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>158</v>
+        <v>773</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>159</v>
+        <v>582</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>160</v>
+        <v>774</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>161</v>
+        <v>775</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>162</v>
+        <v>776</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>163</v>
+        <v>777</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>221</v>
+        <v>161</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="B336" s="4" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="B337" s="4" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="B338" s="4" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B339" s="4" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="B340" s="4" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="B341" s="4" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="B342" s="4" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B343" s="4" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="B344" s="4" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B346" s="4" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="B347" s="4" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="B348" s="4" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="B349" s="4" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="B353" s="4" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="B354" s="4" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="B355" s="4" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="B356" s="4" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="B357" s="4" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="B358" s="4" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="B359" s="4" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="B360" s="4" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="B361" s="4" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="B362" s="4" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="B363" s="4" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" s="3" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="B365" s="4" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="B367" s="4" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="B368" s="4" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="B369" s="4" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="B371" s="4" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="B372" s="4" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B373" s="4" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="3" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="B374" s="4" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="B376" s="4" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="B377" s="4" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="B379" s="4" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="B380" s="4" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="B381" s="4" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="B382" s="4" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="B383" s="4" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="B384" s="4" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="B385" s="4" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="B386" s="4" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="B387" s="4" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="B388" s="4" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="B389" s="4" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="B390" s="4" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="B391" s="4" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="B392" s="4" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="B393" s="4" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" s="3" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
       <c r="B394" s="4" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="B395" s="4" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" s="3" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="B396" s="4" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="B397" s="4" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" s="3" t="s">
-        <v>486</v>
+        <v>470</v>
       </c>
       <c r="B398" s="4" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" s="3" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="B399" s="4" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" s="3" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="B401" s="4" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" s="3" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" s="3" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="B403" s="4" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" s="3" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="B404" s="4" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="B405" s="4" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" s="3" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="B406" s="4" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" s="3" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="B407" s="4" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" s="3" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="B408" s="4" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="B409" s="4" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" s="3" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="B410" s="4" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="B411" s="4" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" s="3" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
       <c r="B412" s="4" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" s="3" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" s="3" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
       <c r="B415" s="4" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" s="3" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="B416" s="4" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" s="3" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="B417" s="4" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" s="3" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="B418" s="4" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" s="3" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="3" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" s="3" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" s="3" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="B422" s="4" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" s="3" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
       <c r="B423" s="4" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" s="3" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="B424" s="4" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="425" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="B425" s="5" t="s">
-        <v>786</v>
+        <v>524</v>
+      </c>
+      <c r="B425" s="4" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" s="3" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="B426" s="4" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" s="3" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="B427" s="4" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" s="3" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="B428" s="4" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" s="3" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="B429" s="4" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" s="3" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="B430" s="4" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" s="3" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="B431" s="4" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" s="3" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="B432" s="4" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A433" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="B433" s="4" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>540</v>
+      </c>
+      <c r="B433" s="5" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" s="3" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="B434" s="4" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
-        <v>111</v>
+        <v>543</v>
       </c>
       <c r="B435" s="4" t="s">
-        <v>112</v>
+        <v>544</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
-        <v>113</v>
+        <v>545</v>
       </c>
       <c r="B436" s="4" t="s">
-        <v>114</v>
+        <v>546</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
-        <v>115</v>
+        <v>547</v>
       </c>
       <c r="B437" s="4" t="s">
-        <v>116</v>
+        <v>548</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" s="3" t="s">
-        <v>117</v>
+        <v>549</v>
       </c>
       <c r="B438" s="4" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
-        <v>119</v>
+        <v>551</v>
       </c>
       <c r="B439" s="4" t="s">
-        <v>120</v>
+        <v>552</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" s="3" t="s">
-        <v>121</v>
+        <v>553</v>
       </c>
       <c r="B440" s="4" t="s">
-        <v>122</v>
+        <v>554</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
-        <v>123</v>
+        <v>555</v>
       </c>
       <c r="B441" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A442" s="3" t="s">
-        <v>125</v>
+        <v>557</v>
       </c>
       <c r="B442" s="4" t="s">
-        <v>126</v>
+        <v>558</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B443" s="4" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" s="3" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B444" s="4" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B445" s="4" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B446" s="4" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B447" s="4" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B448" s="4" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B449" s="4" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" s="3" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B450" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" s="3" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B451" s="4" t="s">
-        <v>785</v>
+        <v>128</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B452" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" s="3" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" s="3" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="B454" s="4" t="s">
-        <v>34</v>
+        <v>134</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" s="3" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="B455" s="4" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" s="3" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="B456" s="4" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" s="3" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B457" s="4" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" s="3" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B458" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A459" s="3" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>32</v>
+        <v>785</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" s="3" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" s="3" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="B461" s="4" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B462" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B463" s="4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B464" s="4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B465" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B466" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" s="3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B467" s="4" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" s="3" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B468" s="4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" s="3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B470" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B471" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B472" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B473" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A474" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B474" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A475" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B475" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A476" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B476" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A477" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B477" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A478" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B478" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A479" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B479" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A480" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B480" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A481" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B473" s="4" t="s">
+      <c r="B481" s="4" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B473">
-    <sortCondition ref="A2:A473"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B481">
+    <sortCondition ref="A2:A481"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>